<commit_message>
leetcode: 451 solution added
</commit_message>
<xml_diff>
--- a/MiniProject/MRU_DS_II_Zeta_Python DSA Mini Project - Bytexl Nimbus.xlsx
+++ b/MiniProject/MRU_DS_II_Zeta_Python DSA Mini Project - Bytexl Nimbus.xlsx
@@ -517,9 +517,6 @@
     <t>Not Submitted</t>
   </si>
   <si>
-    <t>Presented</t>
-  </si>
-  <si>
     <t>Reg No</t>
   </si>
   <si>
@@ -563,6 +560,9 @@
   </si>
   <si>
     <t>Not Presented</t>
+  </si>
+  <si>
+    <t>Review</t>
   </si>
 </sst>
 </file>
@@ -790,27 +790,39 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
-  <dxfs count="38">
+  <dxfs count="34">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -821,141 +833,17 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="0"/>
+        <name val="Arial"/>
+        <scheme val="minor"/>
       </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1081,30 +969,104 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="0"/>
-        <name val="Arial"/>
-        <scheme val="minor"/>
+        <color rgb="FF9C0006"/>
       </font>
-      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -1133,9 +1095,9 @@
   </dxfs>
   <tableStyles count="1">
     <tableStyle name="Form responses 1-style" pivot="0" count="3">
-      <tableStyleElement type="headerRow" dxfId="37"/>
-      <tableStyleElement type="firstRowStripe" dxfId="36"/>
-      <tableStyleElement type="secondRowStripe" dxfId="35"/>
+      <tableStyleElement type="headerRow" dxfId="33"/>
+      <tableStyleElement type="firstRowStripe" dxfId="32"/>
+      <tableStyleElement type="secondRowStripe" dxfId="31"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -1150,26 +1112,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Form_Responses1" displayName="Form_Responses1" ref="A1:L33" headerRowDxfId="34" dataDxfId="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Form_Responses1" displayName="Form_Responses1" ref="A1:L33" headerRowDxfId="13" dataDxfId="12">
   <autoFilter ref="A1:L33"/>
   <sortState ref="A2:L33">
     <sortCondition ref="K1:K33"/>
   </sortState>
   <tableColumns count="12">
-    <tableColumn id="1" name="S.No" dataDxfId="32"/>
-    <tableColumn id="2" name="University" dataDxfId="3"/>
-    <tableColumn id="3" name="Department" dataDxfId="2"/>
-    <tableColumn id="4" name="Section" dataDxfId="1"/>
-    <tableColumn id="5" name="Project Title" dataDxfId="31"/>
+    <tableColumn id="1" name="S.No" dataDxfId="11"/>
+    <tableColumn id="2" name="University" dataDxfId="10"/>
+    <tableColumn id="3" name="Department" dataDxfId="9"/>
+    <tableColumn id="4" name="Section" dataDxfId="8"/>
+    <tableColumn id="5" name="Project Title" dataDxfId="7"/>
     <tableColumn id="6" name="Team Member-1 RegNo" dataDxfId="6"/>
-    <tableColumn id="7" name="Team Member-1 Name" dataDxfId="30"/>
+    <tableColumn id="7" name="Team Member-1 Name" dataDxfId="5"/>
     <tableColumn id="8" name="Team Member-2 RegNo" dataDxfId="4"/>
-    <tableColumn id="9" name="Team Member-2 Name" dataDxfId="5"/>
-    <tableColumn id="10" name="Submission" dataDxfId="8">
+    <tableColumn id="9" name="Team Member-2 Name" dataDxfId="3"/>
+    <tableColumn id="10" name="Submission" dataDxfId="2">
       <calculatedColumnFormula>UPPER(Form_Responses1[[#This Row],[Team Member-2 RegNo]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Presented" dataDxfId="0"/>
-    <tableColumn id="12" name="Status" dataDxfId="7">
+    <tableColumn id="11" name="Review" dataDxfId="1"/>
+    <tableColumn id="12" name="Status" dataDxfId="0">
       <calculatedColumnFormula>RAND()*50</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1178,15 +1140,15 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C6" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28" tableBorderDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C6" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19" tableBorderDxfId="18">
   <autoFilter ref="A1:C6"/>
   <sortState ref="A2:C16">
-    <sortCondition sortBy="cellColor" ref="B1:B16" dxfId="26"/>
+    <sortCondition sortBy="cellColor" ref="B1:B16" dxfId="17"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" name="S.No" dataDxfId="25"/>
-    <tableColumn id="2" name="Reg No" dataDxfId="24"/>
-    <tableColumn id="3" name="Name" dataDxfId="23"/>
+    <tableColumn id="1" name="S.No" dataDxfId="16"/>
+    <tableColumn id="2" name="Reg No" dataDxfId="15"/>
+    <tableColumn id="3" name="Name" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1395,9 +1357,9 @@
   </sheetPr>
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K6" sqref="K6"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2:J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1445,10 +1407,10 @@
         <v>7</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>165</v>
+        <v>180</v>
       </c>
       <c r="L1" s="15" t="s">
         <v>147</v>
@@ -1483,13 +1445,13 @@
         <v>16</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K2" s="21">
         <v>45728</v>
       </c>
       <c r="L2" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1521,13 +1483,13 @@
         <v>92</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K3" s="21">
         <v>45728</v>
       </c>
       <c r="L3" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1559,13 +1521,13 @@
         <v>56</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K4" s="16">
         <v>45729</v>
       </c>
       <c r="L4" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1597,13 +1559,13 @@
         <v>129</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K5" s="16">
         <v>45729</v>
       </c>
       <c r="L5" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1635,13 +1597,13 @@
         <v>82</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K6" s="16">
         <v>45731</v>
       </c>
       <c r="L6" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1673,13 +1635,13 @@
         <v>31</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K7" s="16">
         <v>45731</v>
       </c>
       <c r="L7" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1711,13 +1673,13 @@
         <v>41</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K8" s="16">
         <v>45733</v>
       </c>
       <c r="L8" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1749,13 +1711,13 @@
         <v>104</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K9" s="16">
         <v>45733</v>
       </c>
       <c r="L9" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1787,13 +1749,13 @@
         <v>26</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K10" s="16">
         <v>45734</v>
       </c>
       <c r="L10" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1825,13 +1787,13 @@
         <v>109</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K11" s="16">
         <v>45734</v>
       </c>
       <c r="L11" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1863,13 +1825,13 @@
         <v>51</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K12" s="16">
         <v>45735</v>
       </c>
       <c r="L12" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1907,7 +1869,7 @@
         <v>45735</v>
       </c>
       <c r="L13" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1945,7 +1907,7 @@
         <v>45736</v>
       </c>
       <c r="L14" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1983,7 +1945,7 @@
         <v>45736</v>
       </c>
       <c r="L15" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2021,7 +1983,7 @@
         <v>45737</v>
       </c>
       <c r="L16" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2053,13 +2015,13 @@
         <v>21</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K17" s="16">
         <v>45737</v>
       </c>
       <c r="L17" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2097,7 +2059,7 @@
         <v>45738</v>
       </c>
       <c r="L18" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2135,7 +2097,7 @@
         <v>45738</v>
       </c>
       <c r="L19" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2167,13 +2129,13 @@
         <v>69</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K20" s="16">
         <v>45740</v>
       </c>
       <c r="L20" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2205,13 +2167,13 @@
         <v>72</v>
       </c>
       <c r="J21" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K21" s="16">
         <v>45740</v>
       </c>
       <c r="L21" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2243,13 +2205,13 @@
         <v>133</v>
       </c>
       <c r="J22" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K22" s="16">
         <v>45741</v>
       </c>
       <c r="L22" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2281,13 +2243,13 @@
         <v>46</v>
       </c>
       <c r="J23" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K23" s="16">
         <v>45741</v>
       </c>
       <c r="L23" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2319,13 +2281,13 @@
         <v>122</v>
       </c>
       <c r="J24" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K24" s="16">
         <v>45742</v>
       </c>
       <c r="L24" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2357,13 +2319,13 @@
         <v>13</v>
       </c>
       <c r="J25" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K25" s="16">
         <v>45742</v>
       </c>
       <c r="L25" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2401,7 +2363,7 @@
         <v>45743</v>
       </c>
       <c r="L26" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2439,7 +2401,7 @@
         <v>45743</v>
       </c>
       <c r="L27" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2477,7 +2439,7 @@
         <v>45744</v>
       </c>
       <c r="L28" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2509,13 +2471,13 @@
         <v>100</v>
       </c>
       <c r="J29" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K29" s="16">
         <v>45744</v>
       </c>
       <c r="L29" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2553,7 +2515,7 @@
         <v>45745</v>
       </c>
       <c r="L30" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2585,13 +2547,13 @@
         <v>87</v>
       </c>
       <c r="J31" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K31" s="16">
         <v>45745</v>
       </c>
       <c r="L31" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2623,13 +2585,13 @@
         <v>36</v>
       </c>
       <c r="J32" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K32" s="16">
         <v>45749</v>
       </c>
       <c r="L32" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="33" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2661,24 +2623,24 @@
         <v>77</v>
       </c>
       <c r="J33" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K33" s="16">
         <v>45749</v>
       </c>
       <c r="L33" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="duplicateValues" dxfId="13" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="30" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="duplicateValues" dxfId="12" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="29" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="1" operator="equal">
       <formula>"Not Submitted"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2695,7 +2657,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C2" sqref="C2:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2711,10 +2673,10 @@
         <v>146</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>166</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2722,10 +2684,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>168</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2733,10 +2695,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="C3" s="12" t="s">
         <v>170</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2744,10 +2706,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="C4" s="12" t="s">
         <v>172</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2755,10 +2717,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="C5" s="13" t="s">
         <v>174</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2766,27 +2728,27 @@
         <v>5</v>
       </c>
       <c r="B6" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="C6" s="14" t="s">
         <v>176</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>177</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="21" priority="1"/>
-    <cfRule type="duplicateValues" dxfId="20" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="27" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="26" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B6">
-    <cfRule type="duplicateValues" dxfId="19" priority="13"/>
-    <cfRule type="duplicateValues" dxfId="18" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B6">
-    <cfRule type="duplicateValues" dxfId="17" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="16" priority="16"/>
-    <cfRule type="duplicateValues" dxfId="15" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="17"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
searching algo: linear, binary, jump search algo are added
</commit_message>
<xml_diff>
--- a/MiniProject/MRU_DS_II_Zeta_Python DSA Mini Project - Bytexl Nimbus.xlsx
+++ b/MiniProject/MRU_DS_II_Zeta_Python DSA Mini Project - Bytexl Nimbus.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="182">
   <si>
     <t>University</t>
   </si>
@@ -563,6 +563,9 @@
   </si>
   <si>
     <t>Review</t>
+  </si>
+  <si>
+    <t>Present</t>
   </si>
 </sst>
 </file>
@@ -634,7 +637,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -644,6 +647,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
       </patternFill>
     </fill>
   </fills>
@@ -716,12 +724,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -784,67 +793,17 @@
     <xf numFmtId="14" fontId="8" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="8" fillId="3" borderId="0" xfId="3" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Accent2" xfId="3" builtinId="33"/>
     <cellStyle name="Accent5" xfId="2" builtinId="45"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="34">
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="0"/>
-        <name val="Arial"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -1039,6 +998,60 @@
       </fill>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="0"/>
+        <name val="Arial"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -1112,26 +1125,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Form_Responses1" displayName="Form_Responses1" ref="A1:L33" headerRowDxfId="13" dataDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Form_Responses1" displayName="Form_Responses1" ref="A1:L33" headerRowDxfId="27" dataDxfId="26">
   <autoFilter ref="A1:L33"/>
   <sortState ref="A2:L33">
     <sortCondition ref="K1:K33"/>
   </sortState>
   <tableColumns count="12">
-    <tableColumn id="1" name="S.No" dataDxfId="11"/>
-    <tableColumn id="2" name="University" dataDxfId="10"/>
-    <tableColumn id="3" name="Department" dataDxfId="9"/>
-    <tableColumn id="4" name="Section" dataDxfId="8"/>
-    <tableColumn id="5" name="Project Title" dataDxfId="7"/>
-    <tableColumn id="6" name="Team Member-1 RegNo" dataDxfId="6"/>
-    <tableColumn id="7" name="Team Member-1 Name" dataDxfId="5"/>
-    <tableColumn id="8" name="Team Member-2 RegNo" dataDxfId="4"/>
-    <tableColumn id="9" name="Team Member-2 Name" dataDxfId="3"/>
-    <tableColumn id="10" name="Submission" dataDxfId="2">
+    <tableColumn id="1" name="S.No" dataDxfId="25"/>
+    <tableColumn id="2" name="University" dataDxfId="24"/>
+    <tableColumn id="3" name="Department" dataDxfId="23"/>
+    <tableColumn id="4" name="Section" dataDxfId="22"/>
+    <tableColumn id="5" name="Project Title" dataDxfId="21"/>
+    <tableColumn id="6" name="Team Member-1 RegNo" dataDxfId="20"/>
+    <tableColumn id="7" name="Team Member-1 Name" dataDxfId="19"/>
+    <tableColumn id="8" name="Team Member-2 RegNo" dataDxfId="18"/>
+    <tableColumn id="9" name="Team Member-2 Name" dataDxfId="17"/>
+    <tableColumn id="10" name="Submission" dataDxfId="16">
       <calculatedColumnFormula>UPPER(Form_Responses1[[#This Row],[Team Member-2 RegNo]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Review" dataDxfId="1"/>
-    <tableColumn id="12" name="Status" dataDxfId="0">
+    <tableColumn id="11" name="Review" dataDxfId="15"/>
+    <tableColumn id="12" name="Status" dataDxfId="14">
       <calculatedColumnFormula>RAND()*50</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1140,15 +1153,15 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C6" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19" tableBorderDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C6" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5" tableBorderDxfId="4">
   <autoFilter ref="A1:C6"/>
   <sortState ref="A2:C16">
-    <sortCondition sortBy="cellColor" ref="B1:B16" dxfId="17"/>
+    <sortCondition sortBy="cellColor" ref="B1:B16" dxfId="3"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" name="S.No" dataDxfId="16"/>
-    <tableColumn id="2" name="Reg No" dataDxfId="15"/>
-    <tableColumn id="3" name="Name" dataDxfId="14"/>
+    <tableColumn id="1" name="S.No" dataDxfId="2"/>
+    <tableColumn id="2" name="Reg No" dataDxfId="1"/>
+    <tableColumn id="3" name="Name" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1359,7 +1372,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2:J3"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1451,7 +1464,7 @@
         <v>45728</v>
       </c>
       <c r="L2" s="16" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1485,7 +1498,7 @@
       <c r="J3" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="K3" s="21">
+      <c r="K3" s="22">
         <v>45728</v>
       </c>
       <c r="L3" s="16" t="s">
@@ -1523,7 +1536,7 @@
       <c r="J4" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="K4" s="16">
+      <c r="K4" s="21">
         <v>45729</v>
       </c>
       <c r="L4" s="16" t="s">
@@ -1561,7 +1574,7 @@
       <c r="J5" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="K5" s="16">
+      <c r="K5" s="21">
         <v>45729</v>
       </c>
       <c r="L5" s="16" t="s">
@@ -2736,19 +2749,19 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="27" priority="1"/>
-    <cfRule type="duplicateValues" dxfId="26" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B6">
-    <cfRule type="duplicateValues" dxfId="25" priority="13"/>
-    <cfRule type="duplicateValues" dxfId="24" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B6">
-    <cfRule type="duplicateValues" dxfId="23" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="22" priority="16"/>
-    <cfRule type="duplicateValues" dxfId="21" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="17"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
leetcode 35 and 875 solutions added
</commit_message>
<xml_diff>
--- a/MiniProject/MRU_DS_II_Zeta_Python DSA Mini Project - Bytexl Nimbus.xlsx
+++ b/MiniProject/MRU_DS_II_Zeta_Python DSA Mini Project - Bytexl Nimbus.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9780"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9780" tabRatio="398"/>
   </bookViews>
   <sheets>
     <sheet name="Registered" sheetId="1" r:id="rId1"/>
@@ -730,7 +730,7 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -796,6 +796,7 @@
     <xf numFmtId="14" fontId="8" fillId="3" borderId="0" xfId="3" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent2" xfId="3" builtinId="33"/>
@@ -803,7 +804,259 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
-  <dxfs count="34">
+  <dxfs count="50">
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -928,76 +1181,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1052,36 +1235,6 @@
       <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFF8F9FA"/>
@@ -1108,9 +1261,9 @@
   </dxfs>
   <tableStyles count="1">
     <tableStyle name="Form responses 1-style" pivot="0" count="3">
-      <tableStyleElement type="headerRow" dxfId="33"/>
-      <tableStyleElement type="firstRowStripe" dxfId="32"/>
-      <tableStyleElement type="secondRowStripe" dxfId="31"/>
+      <tableStyleElement type="headerRow" dxfId="49"/>
+      <tableStyleElement type="firstRowStripe" dxfId="48"/>
+      <tableStyleElement type="secondRowStripe" dxfId="47"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -1125,26 +1278,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Form_Responses1" displayName="Form_Responses1" ref="A1:L33" headerRowDxfId="27" dataDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Form_Responses1" displayName="Form_Responses1" ref="A1:L33" headerRowDxfId="46" dataDxfId="45">
   <autoFilter ref="A1:L33"/>
   <sortState ref="A2:L33">
-    <sortCondition ref="K1:K33"/>
+    <sortCondition ref="A1:A33"/>
   </sortState>
   <tableColumns count="12">
-    <tableColumn id="1" name="S.No" dataDxfId="25"/>
-    <tableColumn id="2" name="University" dataDxfId="24"/>
-    <tableColumn id="3" name="Department" dataDxfId="23"/>
-    <tableColumn id="4" name="Section" dataDxfId="22"/>
-    <tableColumn id="5" name="Project Title" dataDxfId="21"/>
-    <tableColumn id="6" name="Team Member-1 RegNo" dataDxfId="20"/>
-    <tableColumn id="7" name="Team Member-1 Name" dataDxfId="19"/>
-    <tableColumn id="8" name="Team Member-2 RegNo" dataDxfId="18"/>
-    <tableColumn id="9" name="Team Member-2 Name" dataDxfId="17"/>
-    <tableColumn id="10" name="Submission" dataDxfId="16">
+    <tableColumn id="1" name="S.No" dataDxfId="44"/>
+    <tableColumn id="2" name="University" dataDxfId="43"/>
+    <tableColumn id="3" name="Department" dataDxfId="42"/>
+    <tableColumn id="4" name="Section" dataDxfId="41"/>
+    <tableColumn id="5" name="Project Title" dataDxfId="40"/>
+    <tableColumn id="6" name="Team Member-1 RegNo" dataDxfId="39"/>
+    <tableColumn id="7" name="Team Member-1 Name" dataDxfId="38"/>
+    <tableColumn id="8" name="Team Member-2 RegNo" dataDxfId="37"/>
+    <tableColumn id="9" name="Team Member-2 Name" dataDxfId="36"/>
+    <tableColumn id="10" name="Submission" dataDxfId="35">
       <calculatedColumnFormula>UPPER(Form_Responses1[[#This Row],[Team Member-2 RegNo]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Review" dataDxfId="15"/>
-    <tableColumn id="12" name="Status" dataDxfId="14">
+    <tableColumn id="11" name="Review" dataDxfId="34"/>
+    <tableColumn id="12" name="Status" dataDxfId="33">
       <calculatedColumnFormula>RAND()*50</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1153,15 +1306,15 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C6" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5" tableBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C6" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31" tableBorderDxfId="30">
   <autoFilter ref="A1:C6"/>
   <sortState ref="A2:C16">
-    <sortCondition sortBy="cellColor" ref="B1:B16" dxfId="3"/>
+    <sortCondition sortBy="cellColor" ref="B1:B16" dxfId="29"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" name="S.No" dataDxfId="2"/>
-    <tableColumn id="2" name="Reg No" dataDxfId="1"/>
-    <tableColumn id="3" name="Name" dataDxfId="0"/>
+    <tableColumn id="1" name="S.No" dataDxfId="28"/>
+    <tableColumn id="2" name="Reg No" dataDxfId="27"/>
+    <tableColumn id="3" name="Name" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1368,11 +1521,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:L33"/>
+  <dimension ref="A1:L70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomLeft" activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1536,11 +1689,11 @@
       <c r="J4" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="K4" s="21">
+      <c r="K4" s="22">
         <v>45729</v>
       </c>
       <c r="L4" s="16" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1574,11 +1727,11 @@
       <c r="J5" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="K5" s="21">
+      <c r="K5" s="22">
         <v>45729</v>
       </c>
       <c r="L5" s="16" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1612,7 +1765,7 @@
       <c r="J6" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="K6" s="16">
+      <c r="K6" s="21">
         <v>45731</v>
       </c>
       <c r="L6" s="16" t="s">
@@ -1650,7 +1803,7 @@
       <c r="J7" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="K7" s="16">
+      <c r="K7" s="21">
         <v>45731</v>
       </c>
       <c r="L7" s="16" t="s">
@@ -1876,7 +2029,7 @@
         <v>140</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>164</v>
+        <v>177</v>
       </c>
       <c r="K13" s="16">
         <v>45735</v>
@@ -1952,7 +2105,7 @@
         <v>61</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>164</v>
+        <v>177</v>
       </c>
       <c r="K15" s="16">
         <v>45736</v>
@@ -1990,7 +2143,7 @@
         <v>114</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>164</v>
+        <v>177</v>
       </c>
       <c r="K16" s="16">
         <v>45737</v>
@@ -2066,7 +2219,7 @@
         <v>142</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>164</v>
+        <v>177</v>
       </c>
       <c r="K18" s="16">
         <v>45738</v>
@@ -2370,7 +2523,7 @@
         <v>95</v>
       </c>
       <c r="J26" s="7" t="s">
-        <v>164</v>
+        <v>177</v>
       </c>
       <c r="K26" s="16">
         <v>45743</v>
@@ -2408,7 +2561,7 @@
         <v>66</v>
       </c>
       <c r="J27" s="7" t="s">
-        <v>164</v>
+        <v>177</v>
       </c>
       <c r="K27" s="16">
         <v>45743</v>
@@ -2522,7 +2675,7 @@
         <v>136</v>
       </c>
       <c r="J30" s="7" t="s">
-        <v>164</v>
+        <v>177</v>
       </c>
       <c r="K30" s="16">
         <v>45745</v>
@@ -2645,16 +2798,132 @@
         <v>179</v>
       </c>
     </row>
+    <row r="35" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H35" s="23"/>
+    </row>
+    <row r="36" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H36" s="23"/>
+    </row>
+    <row r="37" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H37" s="23"/>
+    </row>
+    <row r="38" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H38" s="23"/>
+    </row>
+    <row r="39" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H39" s="23"/>
+    </row>
+    <row r="40" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H40" s="23"/>
+    </row>
+    <row r="41" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H41" s="23"/>
+    </row>
+    <row r="42" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H42" s="23"/>
+    </row>
+    <row r="43" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H43" s="23"/>
+    </row>
+    <row r="44" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H44" s="23"/>
+    </row>
+    <row r="45" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H45" s="23"/>
+    </row>
+    <row r="46" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H46" s="23"/>
+    </row>
+    <row r="47" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H47" s="23"/>
+    </row>
+    <row r="48" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H48" s="23"/>
+    </row>
+    <row r="49" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H49" s="23"/>
+    </row>
+    <row r="50" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H50" s="23"/>
+    </row>
+    <row r="51" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H51" s="23"/>
+    </row>
+    <row r="52" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H52" s="23"/>
+    </row>
+    <row r="53" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H53" s="23"/>
+    </row>
+    <row r="54" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H54" s="23"/>
+    </row>
+    <row r="55" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H55" s="23"/>
+    </row>
+    <row r="56" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H56" s="23"/>
+    </row>
+    <row r="57" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H57" s="23"/>
+    </row>
+    <row r="58" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H58" s="23"/>
+    </row>
+    <row r="59" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H59" s="23"/>
+    </row>
+    <row r="60" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H60" s="23"/>
+    </row>
+    <row r="61" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H61" s="23"/>
+    </row>
+    <row r="62" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H62" s="23"/>
+    </row>
+    <row r="63" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H63" s="23"/>
+    </row>
+    <row r="64" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H64" s="23"/>
+    </row>
+    <row r="65" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H65" s="23"/>
+    </row>
+    <row r="66" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H66" s="23"/>
+    </row>
+    <row r="67" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H67" s="23"/>
+    </row>
+    <row r="68" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H68" s="23"/>
+    </row>
+    <row r="69" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H69" s="23"/>
+    </row>
+    <row r="70" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H70" s="23"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="duplicateValues" dxfId="30" priority="3"/>
+  <conditionalFormatting sqref="H1:H34 H71:H1048576">
+    <cfRule type="duplicateValues" dxfId="8" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="duplicateValues" dxfId="29" priority="2"/>
+  <conditionalFormatting sqref="F1:F34 F71:F1048576">
+    <cfRule type="duplicateValues" dxfId="7" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="cellIs" dxfId="28" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
       <formula>"Not Submitted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1:H1048576">
+    <cfRule type="duplicateValues" dxfId="5" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L1:L1048576">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"Not Presented"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2749,19 +3018,19 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="13" priority="1"/>
-    <cfRule type="duplicateValues" dxfId="12" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B6">
-    <cfRule type="duplicateValues" dxfId="11" priority="13"/>
-    <cfRule type="duplicateValues" dxfId="10" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B6">
-    <cfRule type="duplicateValues" dxfId="9" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="8" priority="16"/>
-    <cfRule type="duplicateValues" dxfId="7" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="17"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Heap: Insertion, Deletion and Sorting using array, linked list, python heapq module are added
</commit_message>
<xml_diff>
--- a/MiniProject/MRU_DS_II_Zeta_Python DSA Mini Project - Bytexl Nimbus.xlsx
+++ b/MiniProject/MRU_DS_II_Zeta_Python DSA Mini Project - Bytexl Nimbus.xlsx
@@ -804,259 +804,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
-  <dxfs count="50">
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="36">
     <dxf>
       <font>
         <strike val="0"/>
@@ -1181,6 +929,76 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1235,6 +1053,56 @@
       <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFF8F9FA"/>
@@ -1261,9 +1129,9 @@
   </dxfs>
   <tableStyles count="1">
     <tableStyle name="Form responses 1-style" pivot="0" count="3">
-      <tableStyleElement type="headerRow" dxfId="49"/>
-      <tableStyleElement type="firstRowStripe" dxfId="48"/>
-      <tableStyleElement type="secondRowStripe" dxfId="47"/>
+      <tableStyleElement type="headerRow" dxfId="35"/>
+      <tableStyleElement type="firstRowStripe" dxfId="34"/>
+      <tableStyleElement type="secondRowStripe" dxfId="33"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -1278,26 +1146,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Form_Responses1" displayName="Form_Responses1" ref="A1:L33" headerRowDxfId="46" dataDxfId="45">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Form_Responses1" displayName="Form_Responses1" ref="A1:L33" headerRowDxfId="27" dataDxfId="26">
   <autoFilter ref="A1:L33"/>
   <sortState ref="A2:L33">
     <sortCondition ref="A1:A33"/>
   </sortState>
   <tableColumns count="12">
-    <tableColumn id="1" name="S.No" dataDxfId="44"/>
-    <tableColumn id="2" name="University" dataDxfId="43"/>
-    <tableColumn id="3" name="Department" dataDxfId="42"/>
-    <tableColumn id="4" name="Section" dataDxfId="41"/>
-    <tableColumn id="5" name="Project Title" dataDxfId="40"/>
-    <tableColumn id="6" name="Team Member-1 RegNo" dataDxfId="39"/>
-    <tableColumn id="7" name="Team Member-1 Name" dataDxfId="38"/>
-    <tableColumn id="8" name="Team Member-2 RegNo" dataDxfId="37"/>
-    <tableColumn id="9" name="Team Member-2 Name" dataDxfId="36"/>
-    <tableColumn id="10" name="Submission" dataDxfId="35">
+    <tableColumn id="1" name="S.No" dataDxfId="25"/>
+    <tableColumn id="2" name="University" dataDxfId="24"/>
+    <tableColumn id="3" name="Department" dataDxfId="23"/>
+    <tableColumn id="4" name="Section" dataDxfId="22"/>
+    <tableColumn id="5" name="Project Title" dataDxfId="21"/>
+    <tableColumn id="6" name="Team Member-1 RegNo" dataDxfId="20"/>
+    <tableColumn id="7" name="Team Member-1 Name" dataDxfId="19"/>
+    <tableColumn id="8" name="Team Member-2 RegNo" dataDxfId="18"/>
+    <tableColumn id="9" name="Team Member-2 Name" dataDxfId="17"/>
+    <tableColumn id="10" name="Submission" dataDxfId="16">
       <calculatedColumnFormula>UPPER(Form_Responses1[[#This Row],[Team Member-2 RegNo]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Review" dataDxfId="34"/>
-    <tableColumn id="12" name="Status" dataDxfId="33">
+    <tableColumn id="11" name="Review" dataDxfId="15"/>
+    <tableColumn id="12" name="Status" dataDxfId="14">
       <calculatedColumnFormula>RAND()*50</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1306,15 +1174,15 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C6" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31" tableBorderDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C6" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5" tableBorderDxfId="4">
   <autoFilter ref="A1:C6"/>
   <sortState ref="A2:C16">
-    <sortCondition sortBy="cellColor" ref="B1:B16" dxfId="29"/>
+    <sortCondition sortBy="cellColor" ref="B1:B16" dxfId="3"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" name="S.No" dataDxfId="28"/>
-    <tableColumn id="2" name="Reg No" dataDxfId="27"/>
-    <tableColumn id="3" name="Name" dataDxfId="26"/>
+    <tableColumn id="1" name="S.No" dataDxfId="2"/>
+    <tableColumn id="2" name="Reg No" dataDxfId="1"/>
+    <tableColumn id="3" name="Name" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1525,7 +1393,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L8" sqref="L8"/>
+      <selection pane="bottomLeft" activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1689,7 +1557,7 @@
       <c r="J4" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="K4" s="22">
+      <c r="K4" s="21">
         <v>45729</v>
       </c>
       <c r="L4" s="16" t="s">
@@ -1727,7 +1595,7 @@
       <c r="J5" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="K5" s="22">
+      <c r="K5" s="21">
         <v>45729</v>
       </c>
       <c r="L5" s="16" t="s">
@@ -1765,7 +1633,7 @@
       <c r="J6" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="K6" s="21">
+      <c r="K6" s="22">
         <v>45731</v>
       </c>
       <c r="L6" s="16" t="s">
@@ -1803,7 +1671,7 @@
       <c r="J7" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="K7" s="21">
+      <c r="K7" s="22">
         <v>45731</v>
       </c>
       <c r="L7" s="16" t="s">
@@ -1841,7 +1709,7 @@
       <c r="J8" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="K8" s="16">
+      <c r="K8" s="22">
         <v>45733</v>
       </c>
       <c r="L8" s="16" t="s">
@@ -1879,7 +1747,7 @@
       <c r="J9" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="K9" s="16">
+      <c r="K9" s="22">
         <v>45733</v>
       </c>
       <c r="L9" s="16" t="s">
@@ -2908,21 +2776,21 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H1:H34 H71:H1048576">
-    <cfRule type="duplicateValues" dxfId="8" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="32" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F34 F71:F1048576">
-    <cfRule type="duplicateValues" dxfId="7" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="31" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="3" operator="equal">
       <formula>"Not Submitted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="duplicateValues" dxfId="5" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="29" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L1048576">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="1" operator="equal">
       <formula>"Not Presented"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3018,19 +2886,19 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="23" priority="1"/>
-    <cfRule type="duplicateValues" dxfId="22" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B6">
-    <cfRule type="duplicateValues" dxfId="21" priority="13"/>
-    <cfRule type="duplicateValues" dxfId="20" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B6">
-    <cfRule type="duplicateValues" dxfId="19" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="18" priority="16"/>
-    <cfRule type="duplicateValues" dxfId="17" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="17"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Leetcode: 621, 1046 added
</commit_message>
<xml_diff>
--- a/MiniProject/MRU_DS_II_Zeta_Python DSA Mini Project - Bytexl Nimbus.xlsx
+++ b/MiniProject/MRU_DS_II_Zeta_Python DSA Mini Project - Bytexl Nimbus.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="178">
   <si>
     <t>University</t>
   </si>
@@ -323,18 +323,6 @@
   </si>
   <si>
     <t xml:space="preserve">V. Chaitanya Kumar </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Warehouse inventory Management </t>
-  </si>
-  <si>
-    <t>Sharvani regula</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2311CS030588 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Soumya panjala </t>
   </si>
   <si>
     <t xml:space="preserve"> Social media Alterrs and messenger</t>
@@ -807,6 +795,126 @@
   <dxfs count="36">
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -929,76 +1037,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1051,56 +1089,6 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -1146,26 +1134,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Form_Responses1" displayName="Form_Responses1" ref="A1:L33" headerRowDxfId="27" dataDxfId="26">
-  <autoFilter ref="A1:L33"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Form_Responses1" displayName="Form_Responses1" ref="A1:L32" headerRowDxfId="32" dataDxfId="31">
+  <autoFilter ref="A1:L32"/>
   <sortState ref="A2:L33">
     <sortCondition ref="A1:A33"/>
   </sortState>
   <tableColumns count="12">
-    <tableColumn id="1" name="S.No" dataDxfId="25"/>
-    <tableColumn id="2" name="University" dataDxfId="24"/>
-    <tableColumn id="3" name="Department" dataDxfId="23"/>
-    <tableColumn id="4" name="Section" dataDxfId="22"/>
-    <tableColumn id="5" name="Project Title" dataDxfId="21"/>
-    <tableColumn id="6" name="Team Member-1 RegNo" dataDxfId="20"/>
-    <tableColumn id="7" name="Team Member-1 Name" dataDxfId="19"/>
-    <tableColumn id="8" name="Team Member-2 RegNo" dataDxfId="18"/>
-    <tableColumn id="9" name="Team Member-2 Name" dataDxfId="17"/>
-    <tableColumn id="10" name="Submission" dataDxfId="16">
+    <tableColumn id="1" name="S.No" dataDxfId="30"/>
+    <tableColumn id="2" name="University" dataDxfId="29"/>
+    <tableColumn id="3" name="Department" dataDxfId="28"/>
+    <tableColumn id="4" name="Section" dataDxfId="27"/>
+    <tableColumn id="5" name="Project Title" dataDxfId="26"/>
+    <tableColumn id="6" name="Team Member-1 RegNo" dataDxfId="25"/>
+    <tableColumn id="7" name="Team Member-1 Name" dataDxfId="24"/>
+    <tableColumn id="8" name="Team Member-2 RegNo" dataDxfId="23"/>
+    <tableColumn id="9" name="Team Member-2 Name" dataDxfId="22"/>
+    <tableColumn id="10" name="Submission" dataDxfId="21">
       <calculatedColumnFormula>UPPER(Form_Responses1[[#This Row],[Team Member-2 RegNo]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Review" dataDxfId="15"/>
-    <tableColumn id="12" name="Status" dataDxfId="14">
+    <tableColumn id="11" name="Review" dataDxfId="20"/>
+    <tableColumn id="12" name="Status" dataDxfId="19">
       <calculatedColumnFormula>RAND()*50</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1174,15 +1162,15 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C6" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5" tableBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C6" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" tableBorderDxfId="16">
   <autoFilter ref="A1:C6"/>
   <sortState ref="A2:C16">
-    <sortCondition sortBy="cellColor" ref="B1:B16" dxfId="3"/>
+    <sortCondition sortBy="cellColor" ref="B1:B16" dxfId="15"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" name="S.No" dataDxfId="2"/>
-    <tableColumn id="2" name="Reg No" dataDxfId="1"/>
-    <tableColumn id="3" name="Name" dataDxfId="0"/>
+    <tableColumn id="1" name="S.No" dataDxfId="14"/>
+    <tableColumn id="2" name="Reg No" dataDxfId="13"/>
+    <tableColumn id="3" name="Name" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1389,11 +1377,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:L70"/>
+  <dimension ref="A1:L69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K11" sqref="K11"/>
+      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1414,7 +1402,7 @@
   <sheetData>
     <row r="1" spans="1:12" s="6" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -1441,13 +1429,13 @@
         <v>7</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="L1" s="15" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1467,25 +1455,25 @@
         <v>14</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="I2" s="19" t="s">
         <v>16</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="K2" s="21">
         <v>45728</v>
       </c>
       <c r="L2" s="16" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1517,13 +1505,13 @@
         <v>92</v>
       </c>
       <c r="J3" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="K3" s="21">
+        <v>45728</v>
+      </c>
+      <c r="L3" s="16" t="s">
         <v>177</v>
-      </c>
-      <c r="K3" s="22">
-        <v>45728</v>
-      </c>
-      <c r="L3" s="16" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1555,13 +1543,13 @@
         <v>56</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="K4" s="21">
         <v>45729</v>
       </c>
       <c r="L4" s="16" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1578,28 +1566,28 @@
         <v>10</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="I5" s="19" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="K5" s="21">
         <v>45729</v>
       </c>
       <c r="L5" s="16" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1631,13 +1619,13 @@
         <v>82</v>
       </c>
       <c r="J6" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="K6" s="21">
+        <v>45731</v>
+      </c>
+      <c r="L6" s="16" t="s">
         <v>177</v>
-      </c>
-      <c r="K6" s="22">
-        <v>45731</v>
-      </c>
-      <c r="L6" s="16" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1669,13 +1657,13 @@
         <v>31</v>
       </c>
       <c r="J7" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="K7" s="21">
+        <v>45731</v>
+      </c>
+      <c r="L7" s="16" t="s">
         <v>177</v>
-      </c>
-      <c r="K7" s="22">
-        <v>45731</v>
-      </c>
-      <c r="L7" s="16" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1707,18 +1695,18 @@
         <v>41</v>
       </c>
       <c r="J8" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="K8" s="21">
+        <v>45733</v>
+      </c>
+      <c r="L8" s="16" t="s">
         <v>177</v>
-      </c>
-      <c r="K8" s="22">
-        <v>45733</v>
-      </c>
-      <c r="L8" s="16" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>8</v>
@@ -1730,33 +1718,33 @@
         <v>10</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>101</v>
+        <v>22</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>81</v>
+        <v>23</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>102</v>
+        <v>24</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>103</v>
+        <v>25</v>
       </c>
       <c r="I9" s="19" t="s">
-        <v>104</v>
+        <v>26</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="K9" s="22">
-        <v>45733</v>
+        <v>45734</v>
       </c>
       <c r="L9" s="16" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>8</v>
@@ -1768,33 +1756,33 @@
         <v>10</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>22</v>
+        <v>101</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>23</v>
+        <v>102</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>24</v>
+        <v>103</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>25</v>
+        <v>104</v>
       </c>
       <c r="I10" s="19" t="s">
-        <v>26</v>
+        <v>105</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="K10" s="16">
+        <v>173</v>
+      </c>
+      <c r="K10" s="22">
         <v>45734</v>
       </c>
       <c r="L10" s="16" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>8</v>
@@ -1806,33 +1794,33 @@
         <v>10</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>105</v>
+        <v>47</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>106</v>
+        <v>48</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>107</v>
+        <v>49</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>108</v>
+        <v>50</v>
       </c>
       <c r="I11" s="19" t="s">
-        <v>109</v>
+        <v>51</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="K11" s="16">
-        <v>45734</v>
+        <v>45735</v>
       </c>
       <c r="L11" s="16" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>8</v>
@@ -1844,33 +1832,33 @@
         <v>10</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>47</v>
+        <v>134</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>48</v>
+        <v>151</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>49</v>
+        <v>135</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>50</v>
+        <v>158</v>
       </c>
       <c r="I12" s="19" t="s">
-        <v>51</v>
+        <v>136</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="K12" s="16">
         <v>45735</v>
       </c>
       <c r="L12" s="16" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>8</v>
@@ -1882,33 +1870,33 @@
         <v>10</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>138</v>
+        <v>111</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>155</v>
+        <v>112</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>139</v>
+        <v>113</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>162</v>
+        <v>114</v>
       </c>
       <c r="I13" s="19" t="s">
-        <v>140</v>
+        <v>115</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
       <c r="K13" s="16">
-        <v>45735</v>
+        <v>45736</v>
       </c>
       <c r="L13" s="16" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>8</v>
@@ -1920,33 +1908,33 @@
         <v>10</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>115</v>
+        <v>57</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>116</v>
+        <v>58</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>117</v>
+        <v>59</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>118</v>
+        <v>60</v>
       </c>
       <c r="I14" s="19" t="s">
-        <v>119</v>
+        <v>61</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="K14" s="16">
         <v>45736</v>
       </c>
       <c r="L14" s="16" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>8</v>
@@ -1958,33 +1946,33 @@
         <v>10</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>57</v>
+        <v>106</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>58</v>
+        <v>107</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>59</v>
+        <v>108</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>60</v>
+        <v>109</v>
       </c>
       <c r="I15" s="19" t="s">
-        <v>61</v>
+        <v>110</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="K15" s="16">
-        <v>45736</v>
+        <v>45737</v>
       </c>
       <c r="L15" s="16" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>8</v>
@@ -1996,33 +1984,33 @@
         <v>10</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>110</v>
+        <v>17</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>111</v>
+        <v>18</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>112</v>
+        <v>19</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>113</v>
+        <v>20</v>
       </c>
       <c r="I16" s="19" t="s">
-        <v>114</v>
+        <v>21</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="K16" s="16">
         <v>45737</v>
       </c>
       <c r="L16" s="16" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>8</v>
@@ -2034,33 +2022,33 @@
         <v>10</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>17</v>
+        <v>137</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>18</v>
+        <v>152</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>19</v>
+        <v>138</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>20</v>
+        <v>152</v>
       </c>
       <c r="I17" s="19" t="s">
-        <v>21</v>
+        <v>138</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="K17" s="16">
-        <v>45737</v>
+        <v>45738</v>
       </c>
       <c r="L17" s="16" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>8</v>
@@ -2072,33 +2060,33 @@
         <v>10</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>142</v>
+        <v>122</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>156</v>
       </c>
       <c r="I18" s="19" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
       <c r="K18" s="16">
         <v>45738</v>
       </c>
       <c r="L18" s="16" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>8</v>
@@ -2110,33 +2098,33 @@
         <v>10</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>125</v>
+        <v>67</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>152</v>
+        <v>91</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>126</v>
+        <v>68</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>160</v>
+        <v>89</v>
       </c>
       <c r="I19" s="19" t="s">
-        <v>127</v>
+        <v>69</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="K19" s="16">
-        <v>45738</v>
+        <v>45740</v>
       </c>
       <c r="L19" s="16" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>8</v>
@@ -2148,33 +2136,33 @@
         <v>10</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>91</v>
+        <v>147</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>89</v>
+        <v>155</v>
       </c>
       <c r="I20" s="19" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="K20" s="16">
         <v>45740</v>
       </c>
       <c r="L20" s="16" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>8</v>
@@ -2186,33 +2174,33 @@
         <v>10</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>70</v>
+        <v>127</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>151</v>
+        <v>126</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>71</v>
+        <v>128</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>159</v>
+        <v>126</v>
       </c>
       <c r="I21" s="19" t="s">
-        <v>72</v>
+        <v>129</v>
       </c>
       <c r="J21" s="7" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="K21" s="16">
-        <v>45740</v>
+        <v>45741</v>
       </c>
       <c r="L21" s="16" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>8</v>
@@ -2224,33 +2212,33 @@
         <v>10</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>131</v>
+        <v>42</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>130</v>
+        <v>43</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>132</v>
+        <v>44</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>130</v>
+        <v>45</v>
       </c>
       <c r="I22" s="19" t="s">
-        <v>133</v>
+        <v>46</v>
       </c>
       <c r="J22" s="7" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="K22" s="16">
         <v>45741</v>
       </c>
       <c r="L22" s="16" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>8</v>
@@ -2262,33 +2250,33 @@
         <v>10</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>42</v>
+        <v>116</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>43</v>
+        <v>119</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>44</v>
+        <v>120</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>45</v>
+        <v>117</v>
       </c>
       <c r="I23" s="19" t="s">
-        <v>46</v>
+        <v>118</v>
       </c>
       <c r="J23" s="7" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="K23" s="16">
-        <v>45741</v>
+        <v>45742</v>
       </c>
       <c r="L23" s="16" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>8</v>
@@ -2300,33 +2288,33 @@
         <v>10</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>120</v>
+        <v>11</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>123</v>
+        <v>144</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>124</v>
+        <v>12</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>121</v>
+        <v>145</v>
       </c>
       <c r="I24" s="19" t="s">
-        <v>122</v>
+        <v>13</v>
       </c>
       <c r="J24" s="7" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="K24" s="16">
         <v>45742</v>
       </c>
       <c r="L24" s="16" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>8</v>
@@ -2338,33 +2326,33 @@
         <v>10</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>11</v>
+        <v>93</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>148</v>
+        <v>65</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>12</v>
+        <v>94</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>149</v>
+        <v>63</v>
       </c>
       <c r="I25" s="19" t="s">
-        <v>13</v>
+        <v>95</v>
       </c>
       <c r="J25" s="7" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="K25" s="16">
-        <v>45742</v>
+        <v>45743</v>
       </c>
       <c r="L25" s="16" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>8</v>
@@ -2376,33 +2364,33 @@
         <v>10</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>93</v>
+        <v>62</v>
       </c>
       <c r="F26" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H26" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="G26" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="I26" s="19" t="s">
-        <v>95</v>
+        <v>66</v>
       </c>
       <c r="J26" s="7" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="K26" s="16">
         <v>45743</v>
       </c>
       <c r="L26" s="16" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>8</v>
@@ -2414,33 +2402,33 @@
         <v>10</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>62</v>
+        <v>139</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>63</v>
+        <v>153</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>64</v>
+        <v>140</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>65</v>
+        <v>159</v>
       </c>
       <c r="I27" s="19" t="s">
-        <v>66</v>
+        <v>141</v>
       </c>
       <c r="J27" s="7" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
       <c r="K27" s="16">
-        <v>45743</v>
+        <v>45744</v>
       </c>
       <c r="L27" s="16" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>8</v>
@@ -2452,33 +2440,33 @@
         <v>10</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>143</v>
+        <v>96</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>157</v>
+        <v>97</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>144</v>
+        <v>98</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>163</v>
+        <v>99</v>
       </c>
       <c r="I28" s="19" t="s">
-        <v>145</v>
+        <v>100</v>
       </c>
       <c r="J28" s="7" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="K28" s="16">
         <v>45744</v>
       </c>
       <c r="L28" s="16" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>8</v>
@@ -2490,33 +2478,33 @@
         <v>10</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>96</v>
+        <v>130</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>97</v>
+        <v>149</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>98</v>
+        <v>131</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>99</v>
+        <v>149</v>
       </c>
       <c r="I29" s="19" t="s">
-        <v>100</v>
+        <v>132</v>
       </c>
       <c r="J29" s="7" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="K29" s="16">
-        <v>45744</v>
+        <v>45745</v>
       </c>
       <c r="L29" s="16" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>8</v>
@@ -2528,33 +2516,33 @@
         <v>10</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>134</v>
+        <v>83</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>153</v>
+        <v>84</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>135</v>
+        <v>85</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>153</v>
+        <v>86</v>
       </c>
       <c r="I30" s="19" t="s">
-        <v>136</v>
+        <v>87</v>
       </c>
       <c r="J30" s="7" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="K30" s="16">
         <v>45745</v>
       </c>
       <c r="L30" s="16" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>8</v>
@@ -2566,33 +2554,33 @@
         <v>10</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>83</v>
+        <v>32</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>84</v>
+        <v>33</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>85</v>
+        <v>34</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>86</v>
+        <v>35</v>
       </c>
       <c r="I31" s="19" t="s">
-        <v>87</v>
+        <v>36</v>
       </c>
       <c r="J31" s="7" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="K31" s="16">
-        <v>45745</v>
+        <v>45749</v>
       </c>
       <c r="L31" s="16" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>8</v>
@@ -2604,108 +2592,73 @@
         <v>10</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>32</v>
+        <v>73</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>33</v>
+        <v>74</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>34</v>
+        <v>75</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>35</v>
+        <v>76</v>
       </c>
       <c r="I32" s="19" t="s">
-        <v>36</v>
+        <v>77</v>
       </c>
       <c r="J32" s="7" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="K32" s="16">
         <v>45749</v>
       </c>
       <c r="L32" s="16" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
-        <v>32</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="I33" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="J33" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="K33" s="16">
-        <v>45749</v>
-      </c>
-      <c r="L33" s="16" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="34" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H34" s="23"/>
+    </row>
+    <row r="35" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H35" s="23"/>
     </row>
-    <row r="36" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H36" s="23"/>
     </row>
-    <row r="37" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H37" s="23"/>
     </row>
-    <row r="38" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H38" s="23"/>
     </row>
-    <row r="39" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H39" s="23"/>
     </row>
-    <row r="40" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H40" s="23"/>
     </row>
-    <row r="41" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H41" s="23"/>
     </row>
-    <row r="42" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H42" s="23"/>
     </row>
-    <row r="43" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H43" s="23"/>
     </row>
-    <row r="44" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H44" s="23"/>
     </row>
-    <row r="45" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H45" s="23"/>
     </row>
-    <row r="46" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H46" s="23"/>
     </row>
-    <row r="47" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H47" s="23"/>
     </row>
-    <row r="48" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H48" s="23"/>
     </row>
     <row r="49" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2771,26 +2724,23 @@
     <row r="69" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H69" s="23"/>
     </row>
-    <row r="70" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H70" s="23"/>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="H1:H34 H71:H1048576">
-    <cfRule type="duplicateValues" dxfId="32" priority="5"/>
+  <conditionalFormatting sqref="H70:H1048576 H1:H33">
+    <cfRule type="duplicateValues" dxfId="11" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F34 F71:F1048576">
-    <cfRule type="duplicateValues" dxfId="31" priority="4"/>
+  <conditionalFormatting sqref="F70:F1048576 F1:F33">
+    <cfRule type="duplicateValues" dxfId="10" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="cellIs" dxfId="30" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
       <formula>"Not Submitted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="duplicateValues" dxfId="29" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L1048576">
-    <cfRule type="cellIs" dxfId="28" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>"Not Presented"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2820,13 +2770,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2834,10 +2784,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2845,10 +2795,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2856,10 +2806,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2867,10 +2817,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2878,27 +2828,27 @@
         <v>5</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="13" priority="1"/>
-    <cfRule type="duplicateValues" dxfId="12" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B6">
-    <cfRule type="duplicateValues" dxfId="11" priority="13"/>
-    <cfRule type="duplicateValues" dxfId="10" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B6">
-    <cfRule type="duplicateValues" dxfId="9" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="8" priority="16"/>
-    <cfRule type="duplicateValues" dxfId="7" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="17"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Dynamic programming material and examples added. leetcode 198 solution added
</commit_message>
<xml_diff>
--- a/MiniProject/MRU_DS_II_Zeta_Python DSA Mini Project - Bytexl Nimbus.xlsx
+++ b/MiniProject/MRU_DS_II_Zeta_Python DSA Mini Project - Bytexl Nimbus.xlsx
@@ -795,126 +795,6 @@
   <dxfs count="36">
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -1037,6 +917,76 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1089,6 +1039,56 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -1134,26 +1134,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Form_Responses1" displayName="Form_Responses1" ref="A1:L32" headerRowDxfId="32" dataDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Form_Responses1" displayName="Form_Responses1" ref="A1:L32" headerRowDxfId="27" dataDxfId="26">
   <autoFilter ref="A1:L32"/>
   <sortState ref="A2:L33">
     <sortCondition ref="A1:A33"/>
   </sortState>
   <tableColumns count="12">
-    <tableColumn id="1" name="S.No" dataDxfId="30"/>
-    <tableColumn id="2" name="University" dataDxfId="29"/>
-    <tableColumn id="3" name="Department" dataDxfId="28"/>
-    <tableColumn id="4" name="Section" dataDxfId="27"/>
-    <tableColumn id="5" name="Project Title" dataDxfId="26"/>
-    <tableColumn id="6" name="Team Member-1 RegNo" dataDxfId="25"/>
-    <tableColumn id="7" name="Team Member-1 Name" dataDxfId="24"/>
-    <tableColumn id="8" name="Team Member-2 RegNo" dataDxfId="23"/>
-    <tableColumn id="9" name="Team Member-2 Name" dataDxfId="22"/>
-    <tableColumn id="10" name="Submission" dataDxfId="21">
+    <tableColumn id="1" name="S.No" dataDxfId="25"/>
+    <tableColumn id="2" name="University" dataDxfId="24"/>
+    <tableColumn id="3" name="Department" dataDxfId="23"/>
+    <tableColumn id="4" name="Section" dataDxfId="22"/>
+    <tableColumn id="5" name="Project Title" dataDxfId="21"/>
+    <tableColumn id="6" name="Team Member-1 RegNo" dataDxfId="20"/>
+    <tableColumn id="7" name="Team Member-1 Name" dataDxfId="19"/>
+    <tableColumn id="8" name="Team Member-2 RegNo" dataDxfId="18"/>
+    <tableColumn id="9" name="Team Member-2 Name" dataDxfId="17"/>
+    <tableColumn id="10" name="Submission" dataDxfId="16">
       <calculatedColumnFormula>UPPER(Form_Responses1[[#This Row],[Team Member-2 RegNo]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Review" dataDxfId="20"/>
-    <tableColumn id="12" name="Status" dataDxfId="19">
+    <tableColumn id="11" name="Review" dataDxfId="15"/>
+    <tableColumn id="12" name="Status" dataDxfId="14">
       <calculatedColumnFormula>RAND()*50</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1162,15 +1162,15 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C6" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" tableBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C6" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5" tableBorderDxfId="4">
   <autoFilter ref="A1:C6"/>
   <sortState ref="A2:C16">
-    <sortCondition sortBy="cellColor" ref="B1:B16" dxfId="15"/>
+    <sortCondition sortBy="cellColor" ref="B1:B16" dxfId="3"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" name="S.No" dataDxfId="14"/>
-    <tableColumn id="2" name="Reg No" dataDxfId="13"/>
-    <tableColumn id="3" name="Name" dataDxfId="12"/>
+    <tableColumn id="1" name="S.No" dataDxfId="2"/>
+    <tableColumn id="2" name="Reg No" dataDxfId="1"/>
+    <tableColumn id="3" name="Name" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1379,9 +1379,9 @@
   </sheetPr>
   <dimension ref="A1:L69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K15" sqref="K15:K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1735,7 +1735,7 @@
       <c r="J9" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="K9" s="22">
+      <c r="K9" s="21">
         <v>45734</v>
       </c>
       <c r="L9" s="16" t="s">
@@ -1773,7 +1773,7 @@
       <c r="J10" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="K10" s="22">
+      <c r="K10" s="21">
         <v>45734</v>
       </c>
       <c r="L10" s="16" t="s">
@@ -1811,7 +1811,7 @@
       <c r="J11" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="K11" s="16">
+      <c r="K11" s="22">
         <v>45735</v>
       </c>
       <c r="L11" s="16" t="s">
@@ -1849,7 +1849,7 @@
       <c r="J12" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="K12" s="16">
+      <c r="K12" s="22">
         <v>45735</v>
       </c>
       <c r="L12" s="16" t="s">
@@ -1887,7 +1887,7 @@
       <c r="J13" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="K13" s="16">
+      <c r="K13" s="22">
         <v>45736</v>
       </c>
       <c r="L13" s="16" t="s">
@@ -1925,7 +1925,7 @@
       <c r="J14" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="K14" s="16">
+      <c r="K14" s="22">
         <v>45736</v>
       </c>
       <c r="L14" s="16" t="s">
@@ -2726,21 +2726,21 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H70:H1048576 H1:H33">
-    <cfRule type="duplicateValues" dxfId="11" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="32" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F70:F1048576 F1:F33">
-    <cfRule type="duplicateValues" dxfId="10" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="31" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="3" operator="equal">
       <formula>"Not Submitted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="duplicateValues" dxfId="8" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="29" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L1048576">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="1" operator="equal">
       <formula>"Not Presented"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2836,19 +2836,19 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="6" priority="1"/>
-    <cfRule type="duplicateValues" dxfId="5" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B6">
-    <cfRule type="duplicateValues" dxfId="4" priority="13"/>
-    <cfRule type="duplicateValues" dxfId="3" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B6">
-    <cfRule type="duplicateValues" dxfId="2" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="1" priority="16"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="17"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>